<commit_message>
resolved War Packing issues
</commit_message>
<xml_diff>
--- a/SW_TC_TS_Generator/DiceSearchJobs/GeneratedTestCases.xlsx
+++ b/SW_TC_TS_Generator/DiceSearchJobs/GeneratedTestCases.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="43">
   <si>
     <t>TC Count</t>
   </si>
@@ -253,21 +253,6 @@
       <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F3" t="s">
-        <v>41</v>
-      </c>
-      <c r="G3" t="s">
-        <v>41</v>
-      </c>
-      <c r="H3" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -279,21 +264,6 @@
       <c r="C4" t="s">
         <v>4</v>
       </c>
-      <c r="D4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F4" t="s">
-        <v>41</v>
-      </c>
-      <c r="G4" t="s">
-        <v>41</v>
-      </c>
-      <c r="H4" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -305,21 +275,6 @@
       <c r="C5" t="s">
         <v>4</v>
       </c>
-      <c r="D5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" t="s">
-        <v>42</v>
-      </c>
-      <c r="F5" t="s">
-        <v>41</v>
-      </c>
-      <c r="G5" t="s">
-        <v>41</v>
-      </c>
-      <c r="H5" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -331,21 +286,6 @@
       <c r="C6" t="s">
         <v>4</v>
       </c>
-      <c r="D6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F6" t="s">
-        <v>41</v>
-      </c>
-      <c r="G6" t="s">
-        <v>41</v>
-      </c>
-      <c r="H6" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -357,21 +297,6 @@
       <c r="C7" t="s">
         <v>4</v>
       </c>
-      <c r="D7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E7" t="s">
-        <v>42</v>
-      </c>
-      <c r="F7" t="s">
-        <v>41</v>
-      </c>
-      <c r="G7" t="s">
-        <v>41</v>
-      </c>
-      <c r="H7" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -383,21 +308,6 @@
       <c r="C8" t="s">
         <v>4</v>
       </c>
-      <c r="D8" t="s">
-        <v>41</v>
-      </c>
-      <c r="E8" t="s">
-        <v>42</v>
-      </c>
-      <c r="F8" t="s">
-        <v>41</v>
-      </c>
-      <c r="G8" t="s">
-        <v>41</v>
-      </c>
-      <c r="H8" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -409,21 +319,6 @@
       <c r="C9" t="s">
         <v>4</v>
       </c>
-      <c r="D9" t="s">
-        <v>41</v>
-      </c>
-      <c r="E9" t="s">
-        <v>42</v>
-      </c>
-      <c r="F9" t="s">
-        <v>41</v>
-      </c>
-      <c r="G9" t="s">
-        <v>41</v>
-      </c>
-      <c r="H9" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -435,21 +330,6 @@
       <c r="C10" t="s">
         <v>4</v>
       </c>
-      <c r="D10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E10" t="s">
-        <v>42</v>
-      </c>
-      <c r="F10" t="s">
-        <v>41</v>
-      </c>
-      <c r="G10" t="s">
-        <v>41</v>
-      </c>
-      <c r="H10" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -461,21 +341,6 @@
       <c r="C11" t="s">
         <v>4</v>
       </c>
-      <c r="D11" t="s">
-        <v>41</v>
-      </c>
-      <c r="E11" t="s">
-        <v>42</v>
-      </c>
-      <c r="F11" t="s">
-        <v>41</v>
-      </c>
-      <c r="G11" t="s">
-        <v>41</v>
-      </c>
-      <c r="H11" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -487,21 +352,6 @@
       <c r="C12" t="s">
         <v>4</v>
       </c>
-      <c r="D12" t="s">
-        <v>41</v>
-      </c>
-      <c r="E12" t="s">
-        <v>42</v>
-      </c>
-      <c r="F12" t="s">
-        <v>41</v>
-      </c>
-      <c r="G12" t="s">
-        <v>41</v>
-      </c>
-      <c r="H12" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -513,21 +363,6 @@
       <c r="C13" t="s">
         <v>4</v>
       </c>
-      <c r="D13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E13" t="s">
-        <v>42</v>
-      </c>
-      <c r="F13" t="s">
-        <v>41</v>
-      </c>
-      <c r="G13" t="s">
-        <v>41</v>
-      </c>
-      <c r="H13" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -539,21 +374,6 @@
       <c r="C14" t="s">
         <v>4</v>
       </c>
-      <c r="D14" t="s">
-        <v>41</v>
-      </c>
-      <c r="E14" t="s">
-        <v>42</v>
-      </c>
-      <c r="F14" t="s">
-        <v>41</v>
-      </c>
-      <c r="G14" t="s">
-        <v>41</v>
-      </c>
-      <c r="H14" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -565,21 +385,6 @@
       <c r="C15" t="s">
         <v>4</v>
       </c>
-      <c r="D15" t="s">
-        <v>41</v>
-      </c>
-      <c r="E15" t="s">
-        <v>42</v>
-      </c>
-      <c r="F15" t="s">
-        <v>41</v>
-      </c>
-      <c r="G15" t="s">
-        <v>41</v>
-      </c>
-      <c r="H15" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -591,21 +396,6 @@
       <c r="C16" t="s">
         <v>4</v>
       </c>
-      <c r="D16" t="s">
-        <v>41</v>
-      </c>
-      <c r="E16" t="s">
-        <v>42</v>
-      </c>
-      <c r="F16" t="s">
-        <v>41</v>
-      </c>
-      <c r="G16" t="s">
-        <v>41</v>
-      </c>
-      <c r="H16" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -616,21 +406,6 @@
       </c>
       <c r="C17" t="s">
         <v>4</v>
-      </c>
-      <c r="D17" t="s">
-        <v>41</v>
-      </c>
-      <c r="E17" t="s">
-        <v>42</v>
-      </c>
-      <c r="F17" t="s">
-        <v>41</v>
-      </c>
-      <c r="G17" t="s">
-        <v>41</v>
-      </c>
-      <c r="H17" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="18">

</xml_diff>